<commit_message>
20241112 temp & wip
</commit_message>
<xml_diff>
--- a/media/caltivation.xlsx
+++ b/media/caltivation.xlsx
@@ -156,8 +156,7 @@
   </si>
   <si>
     <t>基础闪避
-闪避对方下个回合
-10点或以下的攻</t>
+不会受到下一张牌对手消耗灵力的攻的伤害</t>
   </si>
   <si>
     <t>剑修
@@ -1337,7 +1336,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1404,16 +1403,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1423,9 +1416,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1818,7 +1808,7 @@
       <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="34" t="s">
         <v>7</v>
       </c>
       <c r="I1"/>
@@ -1845,612 +1835,612 @@
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="35">
         <v>10</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="35">
         <v>10</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="35">
         <v>10</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="35">
         <v>10</v>
       </c>
-      <c r="F2" s="39">
+      <c r="F2" s="36">
         <v>10</v>
       </c>
-      <c r="G2" s="39">
+      <c r="G2" s="36">
         <f>SUM(B2:F2)</f>
         <v>50</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="35" t="s">
         <v>10</v>
       </c>
       <c r="I2"/>
       <c r="J2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="38">
+      <c r="K2" s="35">
         <v>14</v>
       </c>
-      <c r="L2" s="38">
+      <c r="L2" s="35">
         <v>37</v>
       </c>
-      <c r="M2" s="38">
+      <c r="M2" s="35">
         <v>77</v>
       </c>
-      <c r="N2" s="38">
+      <c r="N2" s="35">
         <v>147</v>
       </c>
-      <c r="O2" s="38"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" ht="21" spans="1:15">
       <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="35">
         <v>10</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="35">
         <v>10</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="35">
         <v>10</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="35">
         <v>10</v>
       </c>
-      <c r="F3" s="39">
+      <c r="F3" s="36">
         <v>10</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="36">
         <f>SUM(B3:F3)</f>
         <v>50</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="35" t="s">
         <v>10</v>
       </c>
       <c r="I3"/>
       <c r="J3" s="14"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
     </row>
     <row r="4" ht="21" spans="1:15">
       <c r="A4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="35">
         <v>9</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="35">
         <v>10</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="35">
         <v>10</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="35">
         <v>10</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="36">
         <v>10</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="36">
         <f t="shared" ref="G4:G10" si="0">SUM(B4:F4)</f>
         <v>49</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="35" t="s">
         <v>10</v>
       </c>
       <c r="I4"/>
       <c r="J4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="41">
+      <c r="K4" s="38">
         <f>K2/B18</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="L4" s="41">
+      <c r="L4" s="38">
         <f>L2/C18</f>
         <v>0.420454545454545</v>
       </c>
-      <c r="M4" s="41">
+      <c r="M4" s="38">
         <f>M2/D18</f>
         <v>0.574626865671642</v>
       </c>
-      <c r="N4" s="41">
+      <c r="N4" s="38">
         <f>N2/E18</f>
         <v>0.816666666666667</v>
       </c>
-      <c r="O4" s="38"/>
+      <c r="O4" s="35"/>
     </row>
     <row r="5" ht="21" spans="1:15">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="36">
         <v>10</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="36">
         <v>10</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="36">
         <v>10</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="36">
         <v>10</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="36">
         <v>10</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="36">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="H5" s="38"/>
+      <c r="H5" s="35"/>
       <c r="I5"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
     </row>
     <row r="6" ht="21" spans="1:15">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="36">
         <v>10</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="36">
         <v>10</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="36">
         <v>10</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="36">
         <v>10</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="36">
         <v>10</v>
       </c>
-      <c r="G6" s="39">
+      <c r="G6" s="36">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="H6" s="38"/>
+      <c r="H6" s="35"/>
       <c r="I6"/>
       <c r="J6"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
     </row>
     <row r="7" ht="21" spans="1:15">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="36">
         <v>10</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="36">
         <v>10</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="36">
         <v>10</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="36">
         <v>10</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="36">
         <v>10</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="36">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="H7" s="38"/>
+      <c r="H7" s="35"/>
       <c r="I7"/>
       <c r="J7"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
     </row>
     <row r="8" ht="21" spans="1:15">
       <c r="A8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="35">
         <v>5</v>
       </c>
-      <c r="C8" s="38">
-        <v>4</v>
-      </c>
-      <c r="D8" s="38">
-        <v>4</v>
-      </c>
-      <c r="E8" s="38">
-        <v>4</v>
-      </c>
-      <c r="F8" s="39">
-        <v>4</v>
-      </c>
-      <c r="G8" s="39">
+      <c r="C8" s="35">
+        <v>4</v>
+      </c>
+      <c r="D8" s="35">
+        <v>4</v>
+      </c>
+      <c r="E8" s="35">
+        <v>4</v>
+      </c>
+      <c r="F8" s="36">
+        <v>4</v>
+      </c>
+      <c r="G8" s="36">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="35" t="s">
         <v>10</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
     </row>
     <row r="9" ht="21" spans="1:15">
       <c r="A9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="38">
-        <v>4</v>
-      </c>
-      <c r="C9" s="38">
-        <v>4</v>
-      </c>
-      <c r="D9" s="38">
-        <v>4</v>
-      </c>
-      <c r="E9" s="38">
-        <v>4</v>
-      </c>
-      <c r="F9" s="39">
-        <v>4</v>
-      </c>
-      <c r="G9" s="39">
+      <c r="B9" s="35">
+        <v>4</v>
+      </c>
+      <c r="C9" s="35">
+        <v>4</v>
+      </c>
+      <c r="D9" s="35">
+        <v>4</v>
+      </c>
+      <c r="E9" s="35">
+        <v>4</v>
+      </c>
+      <c r="F9" s="36">
+        <v>4</v>
+      </c>
+      <c r="G9" s="36">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="35" t="s">
         <v>10</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
     </row>
     <row r="10" ht="21" spans="1:15">
       <c r="A10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="35">
         <v>2</v>
       </c>
-      <c r="C10" s="38">
-        <v>4</v>
-      </c>
-      <c r="D10" s="38">
-        <v>4</v>
-      </c>
-      <c r="E10" s="38">
-        <v>4</v>
-      </c>
-      <c r="F10" s="39">
-        <v>4</v>
-      </c>
-      <c r="G10" s="39">
+      <c r="C10" s="35">
+        <v>4</v>
+      </c>
+      <c r="D10" s="35">
+        <v>4</v>
+      </c>
+      <c r="E10" s="35">
+        <v>4</v>
+      </c>
+      <c r="F10" s="36">
+        <v>4</v>
+      </c>
+      <c r="G10" s="36">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="35" t="s">
         <v>10</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
     </row>
     <row r="11" ht="21" spans="1:15">
       <c r="A11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="38">
+      <c r="B11" s="35">
         <v>2</v>
       </c>
-      <c r="C11" s="38">
-        <v>4</v>
-      </c>
-      <c r="D11" s="38">
-        <v>4</v>
-      </c>
-      <c r="E11" s="38">
-        <v>4</v>
-      </c>
-      <c r="F11" s="39">
-        <v>4</v>
-      </c>
-      <c r="G11" s="39">
+      <c r="C11" s="35">
+        <v>4</v>
+      </c>
+      <c r="D11" s="35">
+        <v>4</v>
+      </c>
+      <c r="E11" s="35">
+        <v>4</v>
+      </c>
+      <c r="F11" s="36">
+        <v>4</v>
+      </c>
+      <c r="G11" s="36">
         <f t="shared" ref="G11:G17" si="1">SUM(B11:F11)</f>
         <v>18</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="35" t="s">
         <v>10</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
     </row>
     <row r="12" ht="21" spans="1:15">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="39">
-        <v>4</v>
-      </c>
-      <c r="C12" s="39">
-        <v>4</v>
-      </c>
-      <c r="D12" s="39">
-        <v>4</v>
-      </c>
-      <c r="E12" s="39">
-        <v>4</v>
-      </c>
-      <c r="F12" s="39">
-        <v>4</v>
-      </c>
-      <c r="G12" s="39">
+      <c r="B12" s="36">
+        <v>4</v>
+      </c>
+      <c r="C12" s="36">
+        <v>4</v>
+      </c>
+      <c r="D12" s="36">
+        <v>4</v>
+      </c>
+      <c r="E12" s="36">
+        <v>4</v>
+      </c>
+      <c r="F12" s="36">
+        <v>4</v>
+      </c>
+      <c r="G12" s="36">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H12" s="38"/>
+      <c r="H12" s="35"/>
       <c r="I12"/>
       <c r="J12"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
     </row>
     <row r="13" ht="21" spans="1:15">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="39">
-        <v>4</v>
-      </c>
-      <c r="C13" s="39">
-        <v>4</v>
-      </c>
-      <c r="D13" s="39">
-        <v>4</v>
-      </c>
-      <c r="E13" s="39">
-        <v>4</v>
-      </c>
-      <c r="F13" s="39">
-        <v>4</v>
-      </c>
-      <c r="G13" s="39">
+      <c r="B13" s="36">
+        <v>4</v>
+      </c>
+      <c r="C13" s="36">
+        <v>4</v>
+      </c>
+      <c r="D13" s="36">
+        <v>4</v>
+      </c>
+      <c r="E13" s="36">
+        <v>4</v>
+      </c>
+      <c r="F13" s="36">
+        <v>4</v>
+      </c>
+      <c r="G13" s="36">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H13" s="38"/>
+      <c r="H13" s="35"/>
       <c r="I13"/>
       <c r="J13"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
     </row>
     <row r="14" ht="21" spans="1:15">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="39">
-        <v>4</v>
-      </c>
-      <c r="C14" s="39">
-        <v>4</v>
-      </c>
-      <c r="D14" s="39">
-        <v>4</v>
-      </c>
-      <c r="E14" s="39">
-        <v>4</v>
-      </c>
-      <c r="F14" s="39">
-        <v>4</v>
-      </c>
-      <c r="G14" s="39">
+      <c r="B14" s="36">
+        <v>4</v>
+      </c>
+      <c r="C14" s="36">
+        <v>4</v>
+      </c>
+      <c r="D14" s="36">
+        <v>4</v>
+      </c>
+      <c r="E14" s="36">
+        <v>4</v>
+      </c>
+      <c r="F14" s="36">
+        <v>4</v>
+      </c>
+      <c r="G14" s="36">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H14" s="38"/>
+      <c r="H14" s="35"/>
       <c r="I14"/>
       <c r="J14"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
     </row>
     <row r="15" ht="21" spans="1:15">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="39">
-        <v>4</v>
-      </c>
-      <c r="C15" s="39">
-        <v>4</v>
-      </c>
-      <c r="D15" s="39">
-        <v>4</v>
-      </c>
-      <c r="E15" s="39">
-        <v>4</v>
-      </c>
-      <c r="F15" s="39">
-        <v>4</v>
-      </c>
-      <c r="G15" s="39">
+      <c r="B15" s="36">
+        <v>4</v>
+      </c>
+      <c r="C15" s="36">
+        <v>4</v>
+      </c>
+      <c r="D15" s="36">
+        <v>4</v>
+      </c>
+      <c r="E15" s="36">
+        <v>4</v>
+      </c>
+      <c r="F15" s="36">
+        <v>4</v>
+      </c>
+      <c r="G15" s="36">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H15" s="38"/>
+      <c r="H15" s="35"/>
       <c r="I15"/>
       <c r="J15"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
     </row>
     <row r="16" ht="21" spans="1:15">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="39">
-        <v>4</v>
-      </c>
-      <c r="C16" s="39">
-        <v>4</v>
-      </c>
-      <c r="D16" s="39">
-        <v>4</v>
-      </c>
-      <c r="E16" s="39">
-        <v>4</v>
-      </c>
-      <c r="F16" s="39">
-        <v>4</v>
-      </c>
-      <c r="G16" s="39">
+      <c r="B16" s="36">
+        <v>4</v>
+      </c>
+      <c r="C16" s="36">
+        <v>4</v>
+      </c>
+      <c r="D16" s="36">
+        <v>4</v>
+      </c>
+      <c r="E16" s="36">
+        <v>4</v>
+      </c>
+      <c r="F16" s="36">
+        <v>4</v>
+      </c>
+      <c r="G16" s="36">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H16" s="38"/>
+      <c r="H16" s="35"/>
       <c r="I16"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="43"/>
-      <c r="O16" s="43"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
     </row>
     <row r="17" ht="21" spans="1:15">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="39">
-        <v>4</v>
-      </c>
-      <c r="C17" s="39">
-        <v>4</v>
-      </c>
-      <c r="D17" s="39">
-        <v>4</v>
-      </c>
-      <c r="E17" s="39">
-        <v>4</v>
-      </c>
-      <c r="F17" s="39">
-        <v>4</v>
-      </c>
-      <c r="G17" s="39">
+      <c r="B17" s="36">
+        <v>4</v>
+      </c>
+      <c r="C17" s="36">
+        <v>4</v>
+      </c>
+      <c r="D17" s="36">
+        <v>4</v>
+      </c>
+      <c r="E17" s="36">
+        <v>4</v>
+      </c>
+      <c r="F17" s="36">
+        <v>4</v>
+      </c>
+      <c r="G17" s="36">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H17" s="38"/>
+      <c r="H17" s="35"/>
       <c r="I17"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
     </row>
     <row r="18" ht="48" customHeight="1" spans="1:15">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="38">
+      <c r="B18" s="35">
         <f>SUM(B2:B4,B8:B11)</f>
         <v>42</v>
       </c>
-      <c r="C18" s="38">
+      <c r="C18" s="35">
         <f>SUM(B2:C4,B8:C11)</f>
         <v>88</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="35">
         <f>SUM(B2:D4,B8:D11)</f>
         <v>134</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="35">
         <f>SUM(B2:E4,B8:E11)</f>
         <v>180</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="35">
         <f>SUM(B2:F4,B8:F11)</f>
         <v>226</v>
       </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
       <c r="I18"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
     </row>
     <row r="19" ht="48" customHeight="1" spans="1:11">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="35">
         <f>SUM(B2:B17)</f>
         <v>96</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="35">
         <f>SUM(B2:C17)</f>
         <v>196</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="35">
         <f>SUM(B2:D17)</f>
         <v>296</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="35">
         <f>SUM(B2:E17)</f>
         <v>396</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="35">
         <f>SUM(B2:F17)</f>
         <v>496</v>
       </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
@@ -2611,7 +2601,7 @@
   <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2703,10 +2693,10 @@
       <c r="I5" s="17"/>
     </row>
     <row r="6" ht="45" spans="1:9">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="19" t="s">
@@ -2720,8 +2710,8 @@
       <c r="I6" s="17"/>
     </row>
     <row r="7" ht="45" spans="1:9">
-      <c r="A7" s="24"/>
-      <c r="B7" s="23"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="19" t="s">
         <v>40</v>
       </c>
@@ -2733,8 +2723,8 @@
       <c r="I7" s="17"/>
     </row>
     <row r="8" ht="45" spans="1:9">
-      <c r="A8" s="24"/>
-      <c r="B8" s="23"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="19" t="s">
         <v>41</v>
       </c>
@@ -2746,8 +2736,8 @@
       <c r="I8" s="17"/>
     </row>
     <row r="9" ht="20.25" spans="1:9">
-      <c r="A9" s="25"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="19" t="s">
@@ -2759,8 +2749,8 @@
       <c r="I9" s="17"/>
     </row>
     <row r="10" ht="45" spans="1:9">
-      <c r="A10" s="25"/>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="18" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -2774,8 +2764,8 @@
       <c r="I10" s="17"/>
     </row>
     <row r="11" ht="30" spans="1:9">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19" t="s">
@@ -2787,8 +2777,8 @@
       <c r="I11" s="17"/>
     </row>
     <row r="12" ht="20.25" spans="1:9">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -2798,8 +2788,8 @@
       <c r="I12" s="17"/>
     </row>
     <row r="13" ht="20.25" spans="1:9">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
@@ -2809,8 +2799,8 @@
       <c r="I13" s="17"/>
     </row>
     <row r="14" ht="30" spans="1:9">
-      <c r="A14" s="25"/>
-      <c r="B14" s="27" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="19" t="s">
@@ -2824,8 +2814,8 @@
       <c r="I14" s="17"/>
     </row>
     <row r="15" ht="30" spans="1:9">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="19" t="s">
         <v>48</v>
       </c>
@@ -2837,8 +2827,8 @@
       <c r="I15" s="17"/>
     </row>
     <row r="16" ht="20.25" spans="1:9">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19" t="s">
@@ -2850,8 +2840,8 @@
       <c r="I16" s="17"/>
     </row>
     <row r="17" ht="20.25" spans="1:9">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19" t="s">
@@ -2863,8 +2853,8 @@
       <c r="I17" s="17"/>
     </row>
     <row r="18" ht="30" spans="1:9">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19" t="s">
@@ -2876,8 +2866,8 @@
       <c r="I18" s="17"/>
     </row>
     <row r="19" ht="30" spans="1:15">
-      <c r="A19" s="25"/>
-      <c r="B19" s="24" t="s">
+      <c r="A19" s="23"/>
+      <c r="B19" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -2899,8 +2889,8 @@
       <c r="O19"/>
     </row>
     <row r="20" ht="45" spans="1:17">
-      <c r="A20" s="25"/>
-      <c r="B20" s="24"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="19" t="s">
         <v>55</v>
       </c>
@@ -2920,8 +2910,8 @@
       <c r="Q20"/>
     </row>
     <row r="21" ht="20.25" spans="1:17">
-      <c r="A21" s="25"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
@@ -2939,8 +2929,8 @@
       <c r="Q21"/>
     </row>
     <row r="22" ht="20.25" spans="1:17">
-      <c r="A22" s="25"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19" t="s">
@@ -2960,8 +2950,8 @@
       <c r="Q22"/>
     </row>
     <row r="23" ht="30" spans="1:17">
-      <c r="A23" s="25"/>
-      <c r="B23" s="27" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="25" t="s">
         <v>57</v>
       </c>
       <c r="C23" s="19" t="s">
@@ -2983,15 +2973,15 @@
       <c r="Q23"/>
     </row>
     <row r="24" ht="45" spans="1:17">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="19" t="s">
         <v>59</v>
       </c>
       <c r="D24" s="19"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
       <c r="H24" s="17"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -3004,15 +2994,15 @@
       <c r="Q24"/>
     </row>
     <row r="25" ht="20.25" spans="1:17">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="17"/>
       <c r="I25"/>
       <c r="J25"/>
@@ -3025,8 +3015,8 @@
       <c r="Q25"/>
     </row>
     <row r="26" ht="30" spans="1:17">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
       <c r="E26" s="19" t="s">
@@ -3050,10 +3040,10 @@
       <c r="Q26"/>
     </row>
     <row r="27" ht="60" spans="1:17">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="20" t="s">
         <v>65</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -3075,8 +3065,8 @@
       <c r="Q27"/>
     </row>
     <row r="28" ht="45" spans="1:17">
-      <c r="A28" s="24"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="19" t="s">
         <v>67</v>
       </c>
@@ -3096,8 +3086,8 @@
       <c r="Q28"/>
     </row>
     <row r="29" ht="20.25" spans="1:17">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24" t="s">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20" t="s">
         <v>68</v>
       </c>
       <c r="C29" s="19"/>
@@ -3117,8 +3107,8 @@
       <c r="Q29"/>
     </row>
     <row r="30" ht="60" spans="1:17">
-      <c r="A30" s="24"/>
-      <c r="B30" s="29"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="19" t="s">
         <v>69</v>
       </c>
@@ -3138,8 +3128,8 @@
       <c r="Q30"/>
     </row>
     <row r="31" ht="75" spans="1:17">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24" t="s">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="19" t="s">
@@ -3161,8 +3151,8 @@
       <c r="Q31"/>
     </row>
     <row r="32" ht="60" spans="1:17">
-      <c r="A32" s="24"/>
-      <c r="B32" s="29"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="21"/>
       <c r="C32" s="19" t="s">
         <v>72</v>
       </c>
@@ -3182,8 +3172,8 @@
       <c r="Q32"/>
     </row>
     <row r="33" ht="45" spans="1:9">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24" t="s">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20" t="s">
         <v>73</v>
       </c>
       <c r="C33" s="19" t="s">
@@ -3197,8 +3187,8 @@
       <c r="I33" s="17"/>
     </row>
     <row r="34" ht="60" spans="1:9">
-      <c r="A34" s="24"/>
-      <c r="B34" s="29"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="21"/>
       <c r="C34" s="19" t="s">
         <v>75</v>
       </c>
@@ -3210,8 +3200,8 @@
       <c r="I34" s="17"/>
     </row>
     <row r="35" ht="60" spans="1:9">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24" t="s">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20" t="s">
         <v>76</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -3225,8 +3215,8 @@
       <c r="I35" s="17"/>
     </row>
     <row r="36" ht="20.25" spans="1:9">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
@@ -3236,11 +3226,11 @@
       <c r="I36" s="17"/>
     </row>
     <row r="37" ht="30" spans="1:9">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="28" t="s">
+      <c r="B37" s="28"/>
+      <c r="C37" s="26" t="s">
         <v>79</v>
       </c>
       <c r="D37" s="19"/>
@@ -3251,40 +3241,40 @@
       <c r="I37" s="17"/>
     </row>
     <row r="38" ht="30" spans="1:9">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="28" t="s">
+      <c r="B38" s="28"/>
+      <c r="C38" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" ht="30" spans="1:9">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="28" t="s">
+      <c r="B39" s="28"/>
+      <c r="C39" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
     </row>
     <row r="40" ht="30" spans="1:9">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="33"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="19" t="s">
         <v>83</v>
       </c>
@@ -3296,8 +3286,8 @@
       <c r="I40" s="17"/>
     </row>
     <row r="41" ht="30" spans="1:9">
-      <c r="A41" s="34"/>
-      <c r="B41" s="33"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="19" t="s">
         <v>84</v>
       </c>
@@ -3309,8 +3299,8 @@
       <c r="I41" s="17"/>
     </row>
     <row r="42" ht="30" spans="1:9">
-      <c r="A42" s="34"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="19" t="s">
         <v>85</v>
       </c>
@@ -3322,8 +3312,8 @@
       <c r="I42" s="17"/>
     </row>
     <row r="43" ht="45" spans="1:9">
-      <c r="A43" s="34"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="31"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="19" t="s">
         <v>86</v>
       </c>
@@ -3335,8 +3325,8 @@
       <c r="I43" s="17"/>
     </row>
     <row r="44" ht="30" spans="1:9">
-      <c r="A44" s="35"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="19" t="s">
         <v>87</v>
       </c>
@@ -3348,10 +3338,10 @@
       <c r="I44" s="17"/>
     </row>
     <row r="45" ht="45" spans="1:9">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="33"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="19" t="s">
         <v>89</v>
       </c>
@@ -3363,8 +3353,8 @@
       <c r="I45" s="17"/>
     </row>
     <row r="46" ht="60" spans="1:9">
-      <c r="A46" s="34"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="31"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="19" t="s">
         <v>90</v>
       </c>
@@ -3376,8 +3366,8 @@
       <c r="I46" s="17"/>
     </row>
     <row r="47" ht="45" spans="1:9">
-      <c r="A47" s="34"/>
-      <c r="B47" s="33"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="19" t="s">
         <v>91</v>
       </c>
@@ -3389,8 +3379,8 @@
       <c r="I47" s="17"/>
     </row>
     <row r="48" ht="75" spans="1:9">
-      <c r="A48" s="35"/>
-      <c r="B48" s="33"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="19" t="s">
         <v>92</v>
       </c>
@@ -3402,10 +3392,10 @@
       <c r="I48" s="17"/>
     </row>
     <row r="49" ht="60" spans="1:9">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="33"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="19" t="s">
         <v>94</v>
       </c>
@@ -3417,8 +3407,8 @@
       <c r="I49" s="17"/>
     </row>
     <row r="50" ht="45" spans="1:9">
-      <c r="A50" s="34"/>
-      <c r="B50" s="33"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="30"/>
       <c r="C50" s="19" t="s">
         <v>95</v>
       </c>
@@ -3430,8 +3420,8 @@
       <c r="I50" s="17"/>
     </row>
     <row r="51" ht="20.25" spans="1:9">
-      <c r="A51" s="34"/>
-      <c r="B51" s="33"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="30"/>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
@@ -3441,8 +3431,8 @@
       <c r="I51" s="17"/>
     </row>
     <row r="52" ht="20.25" spans="1:9">
-      <c r="A52" s="35"/>
-      <c r="B52" s="33"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
@@ -3452,10 +3442,10 @@
       <c r="I52" s="17"/>
     </row>
     <row r="53" ht="60" spans="1:9">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="33"/>
+      <c r="B53" s="30"/>
       <c r="C53" s="19" t="s">
         <v>97</v>
       </c>
@@ -3467,123 +3457,123 @@
       <c r="I53" s="17"/>
     </row>
     <row r="54" ht="60" spans="1:9">
-      <c r="A54" s="34"/>
-      <c r="B54" s="33"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="30"/>
       <c r="C54" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="28"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
       <c r="H54" s="17"/>
       <c r="I54" s="17"/>
     </row>
     <row r="55" ht="20.25" spans="1:9">
-      <c r="A55" s="34"/>
-      <c r="B55" s="33"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="30"/>
       <c r="C55" s="19"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
       <c r="H55" s="17"/>
       <c r="I55" s="17"/>
     </row>
     <row r="56" ht="20.25" spans="1:9">
-      <c r="A56" s="35"/>
-      <c r="B56" s="33"/>
+      <c r="A56" s="32"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="19"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
       <c r="H56" s="17"/>
       <c r="I56" s="17"/>
     </row>
     <row r="57" ht="30" spans="1:9">
-      <c r="A57" s="30" t="s">
+      <c r="A57" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="31"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="19"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
       <c r="H57" s="17"/>
       <c r="I57" s="17"/>
     </row>
     <row r="58" ht="30" spans="1:9">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="31"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="19"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="28"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
       <c r="H58" s="17"/>
       <c r="I58" s="17"/>
     </row>
     <row r="59" ht="30" spans="1:9">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="31"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="19"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="28"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
       <c r="H59" s="17"/>
       <c r="I59" s="17"/>
     </row>
     <row r="60" ht="30" spans="1:9">
-      <c r="A60" s="30" t="s">
+      <c r="A60" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B60" s="31"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="19"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
       <c r="H60" s="17"/>
       <c r="I60" s="17"/>
     </row>
     <row r="61" ht="30" spans="1:9">
-      <c r="A61" s="30" t="s">
+      <c r="A61" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B61" s="31"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="19"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
     </row>
     <row r="62" ht="30" spans="1:9">
-      <c r="A62" s="30" t="s">
+      <c r="A62" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B62" s="31"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="19"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="28"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
     </row>
     <row r="63" ht="20.25" spans="1:9">
-      <c r="A63" s="36" t="s">
+      <c r="A63" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="36"/>
+      <c r="B63" s="33"/>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
       <c r="E63" s="19"/>

</xml_diff>